<commit_message>
Add trained machine learning modules.
</commit_message>
<xml_diff>
--- a/insurance_client/machine-learning-modules/encoded_data.xlsx
+++ b/insurance_client/machine-learning-modules/encoded_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenyingli/Documents/作业/DB/PROJ/Insurance-Product-Web-App/insurance_client/machine-learning-modules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281FA46A-EC21-D043-A26B-C8C572B5FA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEF21D8-21A8-7241-B4C9-62D93D22BC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-460" yWindow="500" windowWidth="16800" windowHeight="11120" xr2:uid="{FBDC94BC-B0D0-4F4A-9067-B3A0C52D6002}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22700" windowHeight="11120" xr2:uid="{FBDC94BC-B0D0-4F4A-9067-B3A0C52D6002}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -441,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BA24655-AEEC-4444-96ED-C90EAC1B804D}">
   <dimension ref="A1:N500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A527" workbookViewId="0">
-      <selection activeCell="M239" sqref="M239"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -529,7 +529,7 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -617,7 +617,7 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -837,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -881,7 +881,7 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -969,7 +969,7 @@
         <v>1</v>
       </c>
       <c r="M12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -1057,7 +1057,7 @@
         <v>0</v>
       </c>
       <c r="M14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -1277,7 +1277,7 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N19">
         <v>0</v>
@@ -1321,7 +1321,7 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N20">
         <v>0</v>
@@ -1409,7 +1409,7 @@
         <v>0</v>
       </c>
       <c r="M22">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N22">
         <v>0</v>
@@ -1453,7 +1453,7 @@
         <v>0</v>
       </c>
       <c r="M23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N23">
         <v>0</v>
@@ -1541,7 +1541,7 @@
         <v>0</v>
       </c>
       <c r="M25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -1805,7 +1805,7 @@
         <v>0</v>
       </c>
       <c r="M31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N31">
         <v>0</v>
@@ -1937,7 +1937,7 @@
         <v>0</v>
       </c>
       <c r="M34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N34">
         <v>0</v>
@@ -2069,7 +2069,7 @@
         <v>1</v>
       </c>
       <c r="M37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N37">
         <v>1</v>
@@ -2377,7 +2377,7 @@
         <v>1</v>
       </c>
       <c r="M44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N44">
         <v>0</v>
@@ -2421,7 +2421,7 @@
         <v>1</v>
       </c>
       <c r="M45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N45">
         <v>0</v>
@@ -2465,7 +2465,7 @@
         <v>0</v>
       </c>
       <c r="M46">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N46">
         <v>0</v>
@@ -2553,7 +2553,7 @@
         <v>0</v>
       </c>
       <c r="M48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N48">
         <v>0</v>
@@ -2817,7 +2817,7 @@
         <v>0</v>
       </c>
       <c r="M54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N54">
         <v>0</v>
@@ -2905,7 +2905,7 @@
         <v>0</v>
       </c>
       <c r="M56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N56">
         <v>0</v>
@@ -3037,7 +3037,7 @@
         <v>0</v>
       </c>
       <c r="M59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N59">
         <v>0</v>
@@ -3081,7 +3081,7 @@
         <v>0</v>
       </c>
       <c r="M60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N60">
         <v>0</v>
@@ -3169,7 +3169,7 @@
         <v>0</v>
       </c>
       <c r="M62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N62">
         <v>0</v>
@@ -3565,7 +3565,7 @@
         <v>0</v>
       </c>
       <c r="M71">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N71">
         <v>0</v>
@@ -3697,7 +3697,7 @@
         <v>0</v>
       </c>
       <c r="M74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N74">
         <v>0</v>
@@ -3873,7 +3873,7 @@
         <v>0</v>
       </c>
       <c r="M78">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N78">
         <v>0</v>
@@ -3961,7 +3961,7 @@
         <v>1</v>
       </c>
       <c r="M80">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N80">
         <v>0</v>
@@ -4401,7 +4401,7 @@
         <v>0</v>
       </c>
       <c r="M90">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N90">
         <v>0</v>
@@ -4929,7 +4929,7 @@
         <v>0</v>
       </c>
       <c r="M102">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N102">
         <v>0</v>
@@ -5149,7 +5149,7 @@
         <v>0</v>
       </c>
       <c r="M107">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N107">
         <v>0</v>
@@ -5325,7 +5325,7 @@
         <v>0</v>
       </c>
       <c r="M111">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N111">
         <v>0</v>
@@ -5369,7 +5369,7 @@
         <v>0</v>
       </c>
       <c r="M112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N112">
         <v>0</v>
@@ -5501,7 +5501,7 @@
         <v>0</v>
       </c>
       <c r="M115">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N115">
         <v>0</v>
@@ -5633,7 +5633,7 @@
         <v>0</v>
       </c>
       <c r="M118">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N118">
         <v>0</v>
@@ -5809,7 +5809,7 @@
         <v>0</v>
       </c>
       <c r="M122">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N122">
         <v>0</v>
@@ -5853,7 +5853,7 @@
         <v>0</v>
       </c>
       <c r="M123">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N123">
         <v>0</v>
@@ -6029,7 +6029,7 @@
         <v>0</v>
       </c>
       <c r="M127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N127">
         <v>0</v>
@@ -6073,7 +6073,7 @@
         <v>0</v>
       </c>
       <c r="M128">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N128">
         <v>0</v>
@@ -6117,7 +6117,7 @@
         <v>1</v>
       </c>
       <c r="M129">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N129">
         <v>0</v>
@@ -6205,7 +6205,7 @@
         <v>1</v>
       </c>
       <c r="M131">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N131">
         <v>0</v>
@@ -6425,7 +6425,7 @@
         <v>0</v>
       </c>
       <c r="M136">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N136">
         <v>0</v>
@@ -6513,7 +6513,7 @@
         <v>0</v>
       </c>
       <c r="M138">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N138">
         <v>0</v>
@@ -6601,7 +6601,7 @@
         <v>0</v>
       </c>
       <c r="M140">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N140">
         <v>0</v>
@@ -6645,7 +6645,7 @@
         <v>0</v>
       </c>
       <c r="M141">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N141">
         <v>0</v>
@@ -7085,7 +7085,7 @@
         <v>1</v>
       </c>
       <c r="M151">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N151">
         <v>0</v>
@@ -7349,7 +7349,7 @@
         <v>0</v>
       </c>
       <c r="M157">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N157">
         <v>0</v>
@@ -7789,7 +7789,7 @@
         <v>1</v>
       </c>
       <c r="M167">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N167">
         <v>0</v>
@@ -8053,7 +8053,7 @@
         <v>0</v>
       </c>
       <c r="M173">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N173">
         <v>0</v>
@@ -8097,7 +8097,7 @@
         <v>0</v>
       </c>
       <c r="M174">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N174">
         <v>0</v>
@@ -8493,7 +8493,7 @@
         <v>1</v>
       </c>
       <c r="M183">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N183">
         <v>0</v>
@@ -8713,7 +8713,7 @@
         <v>0</v>
       </c>
       <c r="M188">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N188">
         <v>0</v>
@@ -8757,7 +8757,7 @@
         <v>0</v>
       </c>
       <c r="M189">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N189">
         <v>0</v>
@@ -9109,7 +9109,7 @@
         <v>0</v>
       </c>
       <c r="M197">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N197">
         <v>0</v>
@@ -9461,7 +9461,7 @@
         <v>0</v>
       </c>
       <c r="M205">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N205">
         <v>0</v>
@@ -9505,7 +9505,7 @@
         <v>1</v>
       </c>
       <c r="M206">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N206">
         <v>0</v>
@@ -9769,7 +9769,7 @@
         <v>0</v>
       </c>
       <c r="M212">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N212">
         <v>0</v>
@@ -9901,7 +9901,7 @@
         <v>0</v>
       </c>
       <c r="M215">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N215">
         <v>0</v>
@@ -9989,7 +9989,7 @@
         <v>1</v>
       </c>
       <c r="M217">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N217">
         <v>0</v>
@@ -10341,7 +10341,7 @@
         <v>0</v>
       </c>
       <c r="M225">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N225">
         <v>0</v>
@@ -10561,7 +10561,7 @@
         <v>0</v>
       </c>
       <c r="M230">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N230">
         <v>0</v>
@@ -10693,7 +10693,7 @@
         <v>0</v>
       </c>
       <c r="M233">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N233">
         <v>0</v>
@@ -10869,7 +10869,7 @@
         <v>0</v>
       </c>
       <c r="M237">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N237">
         <v>0</v>
@@ -10913,7 +10913,7 @@
         <v>0</v>
       </c>
       <c r="M238">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N238">
         <v>0</v>
@@ -10957,7 +10957,7 @@
         <v>0</v>
       </c>
       <c r="M239">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N239">
         <v>0</v>
@@ -11089,7 +11089,7 @@
         <v>0</v>
       </c>
       <c r="M242">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N242">
         <v>0</v>
@@ -11133,7 +11133,7 @@
         <v>0</v>
       </c>
       <c r="M243">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N243">
         <v>0</v>
@@ -11177,7 +11177,7 @@
         <v>0</v>
       </c>
       <c r="M244">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N244">
         <v>0</v>
@@ -11221,7 +11221,7 @@
         <v>1</v>
       </c>
       <c r="M245">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N245">
         <v>0</v>
@@ -11265,7 +11265,7 @@
         <v>0</v>
       </c>
       <c r="M246">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N246">
         <v>0</v>
@@ -11309,7 +11309,7 @@
         <v>1</v>
       </c>
       <c r="M247">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N247">
         <v>0</v>
@@ -11617,7 +11617,7 @@
         <v>0</v>
       </c>
       <c r="M254">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N254">
         <v>0</v>
@@ -11705,7 +11705,7 @@
         <v>0</v>
       </c>
       <c r="M256">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N256">
         <v>0</v>
@@ -12277,7 +12277,7 @@
         <v>0</v>
       </c>
       <c r="M269">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N269">
         <v>0</v>
@@ -12321,7 +12321,7 @@
         <v>0</v>
       </c>
       <c r="M270">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N270">
         <v>0</v>
@@ -12409,7 +12409,7 @@
         <v>1</v>
       </c>
       <c r="M272">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N272">
         <v>1</v>
@@ -12585,7 +12585,7 @@
         <v>0</v>
       </c>
       <c r="M276">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N276">
         <v>0</v>
@@ -12673,7 +12673,7 @@
         <v>0</v>
       </c>
       <c r="M278">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N278">
         <v>0</v>
@@ -12805,7 +12805,7 @@
         <v>1</v>
       </c>
       <c r="M281">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N281">
         <v>1</v>
@@ -12893,7 +12893,7 @@
         <v>1</v>
       </c>
       <c r="M283">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N283">
         <v>0</v>
@@ -13113,7 +13113,7 @@
         <v>1</v>
       </c>
       <c r="M288">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N288">
         <v>0</v>
@@ -13421,7 +13421,7 @@
         <v>1</v>
       </c>
       <c r="M295">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N295">
         <v>0</v>
@@ -13685,7 +13685,7 @@
         <v>0</v>
       </c>
       <c r="M301">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N301">
         <v>1</v>
@@ -13729,7 +13729,7 @@
         <v>0</v>
       </c>
       <c r="M302">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N302">
         <v>0</v>
@@ -13993,7 +13993,7 @@
         <v>1</v>
       </c>
       <c r="M308">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N308">
         <v>1</v>
@@ -14037,7 +14037,7 @@
         <v>0</v>
       </c>
       <c r="M309">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N309">
         <v>0</v>
@@ -14301,7 +14301,7 @@
         <v>0</v>
       </c>
       <c r="M315">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N315">
         <v>0</v>
@@ -14345,7 +14345,7 @@
         <v>0</v>
       </c>
       <c r="M316">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N316">
         <v>0</v>
@@ -14565,7 +14565,7 @@
         <v>0</v>
       </c>
       <c r="M321">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N321">
         <v>0</v>
@@ -14873,7 +14873,7 @@
         <v>0</v>
       </c>
       <c r="M328">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N328">
         <v>0</v>
@@ -15049,7 +15049,7 @@
         <v>0</v>
       </c>
       <c r="M332">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N332">
         <v>1</v>
@@ -15137,7 +15137,7 @@
         <v>0</v>
       </c>
       <c r="M334">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N334">
         <v>0</v>
@@ -15181,7 +15181,7 @@
         <v>0</v>
       </c>
       <c r="M335">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N335">
         <v>0</v>
@@ -15269,7 +15269,7 @@
         <v>0</v>
       </c>
       <c r="M337">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N337">
         <v>0</v>
@@ -15489,7 +15489,7 @@
         <v>0</v>
       </c>
       <c r="M342">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N342">
         <v>0</v>
@@ -15577,7 +15577,7 @@
         <v>0</v>
       </c>
       <c r="M344">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N344">
         <v>0</v>
@@ -15621,7 +15621,7 @@
         <v>0</v>
       </c>
       <c r="M345">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N345">
         <v>0</v>
@@ -15753,7 +15753,7 @@
         <v>1</v>
       </c>
       <c r="M348">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N348">
         <v>0</v>
@@ -15797,7 +15797,7 @@
         <v>0</v>
       </c>
       <c r="M349">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N349">
         <v>0</v>
@@ -15885,7 +15885,7 @@
         <v>1</v>
       </c>
       <c r="M351">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N351">
         <v>0</v>
@@ -16413,7 +16413,7 @@
         <v>0</v>
       </c>
       <c r="M363">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N363">
         <v>0</v>
@@ -16457,7 +16457,7 @@
         <v>0</v>
       </c>
       <c r="M364">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N364">
         <v>0</v>
@@ -16545,7 +16545,7 @@
         <v>0</v>
       </c>
       <c r="M366">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N366">
         <v>0</v>
@@ -16721,7 +16721,7 @@
         <v>0</v>
       </c>
       <c r="M370">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N370">
         <v>0</v>
@@ -16809,7 +16809,7 @@
         <v>1</v>
       </c>
       <c r="M372">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N372">
         <v>1</v>
@@ -17161,7 +17161,7 @@
         <v>1</v>
       </c>
       <c r="M380">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N380">
         <v>1</v>
@@ -17293,7 +17293,7 @@
         <v>1</v>
       </c>
       <c r="M383">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N383">
         <v>0</v>
@@ -17557,7 +17557,7 @@
         <v>0</v>
       </c>
       <c r="M389">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N389">
         <v>0</v>
@@ -17601,7 +17601,7 @@
         <v>0</v>
       </c>
       <c r="M390">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N390">
         <v>0</v>
@@ -17865,7 +17865,7 @@
         <v>0</v>
       </c>
       <c r="M396">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N396">
         <v>0</v>
@@ -18041,7 +18041,7 @@
         <v>0</v>
       </c>
       <c r="M400">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N400">
         <v>0</v>
@@ -18173,7 +18173,7 @@
         <v>0</v>
       </c>
       <c r="M403">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N403">
         <v>0</v>
@@ -18217,7 +18217,7 @@
         <v>0</v>
       </c>
       <c r="M404">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N404">
         <v>0</v>
@@ -18305,7 +18305,7 @@
         <v>1</v>
       </c>
       <c r="M406">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N406">
         <v>0</v>
@@ -18393,7 +18393,7 @@
         <v>0</v>
       </c>
       <c r="M408">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N408">
         <v>1</v>
@@ -18569,7 +18569,7 @@
         <v>1</v>
       </c>
       <c r="M412">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N412">
         <v>1</v>
@@ -18613,7 +18613,7 @@
         <v>0</v>
       </c>
       <c r="M413">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N413">
         <v>0</v>
@@ -18745,7 +18745,7 @@
         <v>0</v>
       </c>
       <c r="M416">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N416">
         <v>0</v>
@@ -18789,7 +18789,7 @@
         <v>0</v>
       </c>
       <c r="M417">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N417">
         <v>0</v>
@@ -18877,7 +18877,7 @@
         <v>1</v>
       </c>
       <c r="M419">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N419">
         <v>1</v>
@@ -18921,7 +18921,7 @@
         <v>1</v>
       </c>
       <c r="M420">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N420">
         <v>0</v>
@@ -19141,7 +19141,7 @@
         <v>0</v>
       </c>
       <c r="M425">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N425">
         <v>0</v>
@@ -19185,7 +19185,7 @@
         <v>0</v>
       </c>
       <c r="M426">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N426">
         <v>0</v>
@@ -19493,7 +19493,7 @@
         <v>0</v>
       </c>
       <c r="M433">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N433">
         <v>0</v>
@@ -19669,7 +19669,7 @@
         <v>0</v>
       </c>
       <c r="M437">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N437">
         <v>0</v>
@@ -19801,7 +19801,7 @@
         <v>0</v>
       </c>
       <c r="M440">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N440">
         <v>0</v>
@@ -20109,7 +20109,7 @@
         <v>0</v>
       </c>
       <c r="M447">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N447">
         <v>0</v>
@@ -20549,7 +20549,7 @@
         <v>1</v>
       </c>
       <c r="M457">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N457">
         <v>0</v>
@@ -20637,7 +20637,7 @@
         <v>1</v>
       </c>
       <c r="M459">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N459">
         <v>1</v>
@@ -20681,7 +20681,7 @@
         <v>0</v>
       </c>
       <c r="M460">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N460">
         <v>0</v>
@@ -20901,7 +20901,7 @@
         <v>0</v>
       </c>
       <c r="M465">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N465">
         <v>0</v>
@@ -20989,7 +20989,7 @@
         <v>0</v>
       </c>
       <c r="M467">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N467">
         <v>0</v>
@@ -21165,7 +21165,7 @@
         <v>1</v>
       </c>
       <c r="M471">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N471">
         <v>1</v>
@@ -22045,7 +22045,7 @@
         <v>0</v>
       </c>
       <c r="M491">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N491">
         <v>0</v>
@@ -22089,7 +22089,7 @@
         <v>0</v>
       </c>
       <c r="M492">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N492">
         <v>0</v>

</xml_diff>